<commit_message>
Sistema de diretoria implementado
</commit_message>
<xml_diff>
--- a/db/logins.xlsx
+++ b/db/logins.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eurico.dante\Desktop\testes-programação\entrada-manutenção\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\eurico.dante\Desktop\testes-programação\entrada-manutenção v0.2\db\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1EF2B607-2FDD-40BB-90D2-473690ECA49E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C6B682CA-E986-4122-B982-B02C3345D447}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -378,10 +378,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B6"/>
+  <dimension ref="A1:B7"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F7" sqref="F7"/>
+      <selection activeCell="B7" sqref="B7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -438,6 +438,14 @@
         <v>18051980</v>
       </c>
     </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A7">
+        <v>1</v>
+      </c>
+      <c r="B7">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>